<commit_message>
change for unsder staing
</commit_message>
<xml_diff>
--- a/bug/redmine/template.xlsx
+++ b/bug/redmine/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\bug\redmine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F47C04-5DEC-4A12-A640-A7EC720D65C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8311D5-10E5-49C5-83FB-6CEAD58827C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Jira Task No: 1419 </t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>SYM1419-001</t>
+  </si>
+  <si>
+    <t>2. goto seeting</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -966,7 +969,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1127,7 +1130,9 @@
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>

</xml_diff>